<commit_message>
Appliy Card Styling + Update translations
</commit_message>
<xml_diff>
--- a/TherapyHessen/doc/Translation-Therapy-Hessen.xlsx
+++ b/TherapyHessen/doc/Translation-Therapy-Hessen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Trunk\Samples\TherapyHessen\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9875BBF0-7721-4CB7-8460-2612B8721F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5BE5C6-08C9-4CD1-899C-BAFC7B651DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1440" windowWidth="38640" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="185">
   <si>
     <t>Turkish</t>
   </si>
@@ -552,13 +552,50 @@
   </si>
   <si>
     <t>);</t>
+  </si>
+  <si>
+    <t>Çocuk Terapisi</t>
+  </si>
+  <si>
+    <t>Kindertherapy</t>
+  </si>
+  <si>
+    <t>Jugendliche Therapy</t>
+  </si>
+  <si>
+    <t>Ergen Terapisi</t>
+  </si>
+  <si>
+    <t>Oyun; çocuğun kendini ifade etmesi, hayal ile gerçek arasında bir köprü, gizli enerjinin kullanılması, çocuğun sosyal ve ahlaki değerleri öğrendiği bir alandır.</t>
+  </si>
+  <si>
+    <t>Spiel; ist ein Bereich, in dem das Kind sich selbst ausdrückt, eine Brücke zwischen Phantasie und Realität, die Nutzung verborgener Energien, und in dem das Kind soziale und moralische Werte erlernt.</t>
+  </si>
+  <si>
+    <t>Es ist notwendig, mit Kindern im Alter von 3-11 Jahren zu kommunizieren, indem man Methoden verwendet, mit denen sie sich besser ausdrücken können.
+In dieser Zeit ist die Analyse der inneren Welt des Kindes anhand der Zeichnungen leicht möglich. Anhand dieser Zeichnungen lassen sich die Bedürfnisse des Kindes ermitteln.</t>
+  </si>
+  <si>
+    <t>3-11 yaş çocukları ile kendilerini daha iyi ifade edebilecekleri yöntemler kullanılarak iletişim kurmak gereklidir. Bu dönemde çocuğun iç dünyasının analiz edilmesi çizdiği resimler yoluyla kolayca mümkün olmaktadır. Bu çizimler sonucunda çocuğun ihtiyaçları belirlenebilmektedir.</t>
+  </si>
+  <si>
+    <t>child_drawing_info_1</t>
+  </si>
+  <si>
+    <t>teenager_section_sub_title</t>
+  </si>
+  <si>
+    <t>game_therapy_info_1</t>
+  </si>
+  <si>
+    <t>child_section_sub_title</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -589,6 +626,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -659,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -672,6 +725,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -890,10 +961,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -907,20 +978,20 @@
     <col min="7" max="7" width="87.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C1" s="3" t="s">
+    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="11" t="s">
         <v>169</v>
       </c>
     </row>
@@ -1158,7 +1229,7 @@
       <c r="B12" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>106</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1177,988 +1248,1082 @@
         <v>$("[data-lang=contact_section_title]").text(language.contact_section_title);</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>4</v>
+      <c r="B13" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>174</v>
       </c>
       <c r="E13" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B13,Sheet2!B$3,C13,Sheet2!B$4)</f>
-        <v>"child_list_item_1": "Uyku Sorunları",</v>
+        <v>"child_section_sub_title": "Çocuk Terapisi",</v>
       </c>
       <c r="F13" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B13,Sheet2!B$3,D13,Sheet2!B$4)</f>
-        <v>"child_list_item_1": "Schlafprobleme",</v>
+        <v>"child_section_sub_title": "Kindertherapy",</v>
       </c>
       <c r="G13" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B13,Sheet2!B$7,B13,Sheet2!B$8)</f>
-        <v>$("[data-lang=child_list_item_1]").text(language.child_list_item_1);</v>
+        <v>$("[data-lang=child_section_sub_title]").text(language.child_section_sub_title);</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
       <c r="B14" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E14" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B14,Sheet2!B$3,C14,Sheet2!B$4)</f>
-        <v>"child_list_item_2": "Yeme Sorunları",</v>
+        <v>"child_list_item_1": "Uyku Sorunları",</v>
       </c>
       <c r="F14" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B14,Sheet2!B$3,D14,Sheet2!B$4)</f>
-        <v>"child_list_item_2": "Probleme beim Essen",</v>
+        <v>"child_list_item_1": "Schlafprobleme",</v>
       </c>
       <c r="G14" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B14,Sheet2!B$7,B14,Sheet2!B$8)</f>
-        <v>$("[data-lang=child_list_item_2]").text(language.child_list_item_2);</v>
+        <v>$("[data-lang=child_list_item_1]").text(language.child_list_item_1);</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E15" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B15,Sheet2!B$3,C15,Sheet2!B$4)</f>
-        <v>"child_list_item_3": "Gelişim Sorunları",</v>
+        <v>"child_list_item_2": "Yeme Sorunları",</v>
       </c>
       <c r="F15" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B15,Sheet2!B$3,D15,Sheet2!B$4)</f>
-        <v>"child_list_item_3": "Entwicklungspolitische Probleme",</v>
+        <v>"child_list_item_2": "Probleme beim Essen",</v>
       </c>
       <c r="G15" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B15,Sheet2!B$7,B15,Sheet2!B$8)</f>
-        <v>$("[data-lang=child_list_item_3]").text(language.child_list_item_3);</v>
+        <v>$("[data-lang=child_list_item_2]").text(language.child_list_item_2);</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E16" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B16,Sheet2!B$3,C16,Sheet2!B$4)</f>
-        <v>"child_list_item_4": "Anne-Baba-Çocuk İletişim Sorunları",</v>
+        <v>"child_list_item_3": "Gelişim Sorunları",</v>
       </c>
       <c r="F16" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B16,Sheet2!B$3,D16,Sheet2!B$4)</f>
-        <v>"child_list_item_4": "Kommunikationsprobleme zwischen Eltern und Kind",</v>
+        <v>"child_list_item_3": "Entwicklungspolitische Probleme",</v>
       </c>
       <c r="G16" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B16,Sheet2!B$7,B16,Sheet2!B$8)</f>
-        <v>$("[data-lang=child_list_item_4]").text(language.child_list_item_4);</v>
+        <v>$("[data-lang=child_list_item_3]").text(language.child_list_item_3);</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E17" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B17,Sheet2!B$3,C17,Sheet2!B$4)</f>
-        <v>"child_list_item_5": "Davranım Bozuklukları",</v>
+        <v>"child_list_item_4": "Anne-Baba-Çocuk İletişim Sorunları",</v>
       </c>
       <c r="F17" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B17,Sheet2!B$3,D17,Sheet2!B$4)</f>
-        <v>"child_list_item_5": "Verhaltensstörungen",</v>
+        <v>"child_list_item_4": "Kommunikationsprobleme zwischen Eltern und Kind",</v>
       </c>
       <c r="G17" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B17,Sheet2!B$7,B17,Sheet2!B$8)</f>
-        <v>$("[data-lang=child_list_item_5]").text(language.child_list_item_5);</v>
+        <v>$("[data-lang=child_list_item_4]").text(language.child_list_item_4);</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E18" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B18,Sheet2!B$3,C18,Sheet2!B$4)</f>
-        <v>"child_list_item_6": "Arkadaş İlişkileri İle İlgili Sorunlar",</v>
+        <v>"child_list_item_5": "Davranım Bozuklukları",</v>
       </c>
       <c r="F18" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B18,Sheet2!B$3,D18,Sheet2!B$4)</f>
-        <v>"child_list_item_6": "Probleme mit Freundschaftsbeziehungen",</v>
+        <v>"child_list_item_5": "Verhaltensstörungen",</v>
       </c>
       <c r="G18" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B18,Sheet2!B$7,B18,Sheet2!B$8)</f>
-        <v>$("[data-lang=child_list_item_6]").text(language.child_list_item_6);</v>
+        <v>$("[data-lang=child_list_item_5]").text(language.child_list_item_5);</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E19" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B19,Sheet2!B$3,C19,Sheet2!B$4)</f>
-        <v>"child_list_item_7": "Kardeş Kıskançlığı",</v>
+        <v>"child_list_item_6": "Arkadaş İlişkileri İle İlgili Sorunlar",</v>
       </c>
       <c r="F19" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B19,Sheet2!B$3,D19,Sheet2!B$4)</f>
-        <v>"child_list_item_7": "Eifersucht unter Geschwistern",</v>
+        <v>"child_list_item_6": "Probleme mit Freundschaftsbeziehungen",</v>
       </c>
       <c r="G19" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B19,Sheet2!B$7,B19,Sheet2!B$8)</f>
-        <v>$("[data-lang=child_list_item_7]").text(language.child_list_item_7);</v>
+        <v>$("[data-lang=child_list_item_6]").text(language.child_list_item_6);</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E20" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B20,Sheet2!B$3,C20,Sheet2!B$4)</f>
-        <v>"child_list_item_8": "Dikkat ve Hiperaktivite Bozukluğu",</v>
+        <v>"child_list_item_7": "Kardeş Kıskançlığı",</v>
       </c>
       <c r="F20" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B20,Sheet2!B$3,D20,Sheet2!B$4)</f>
-        <v>"child_list_item_8": "Aufmerksamkeits- und Hyperaktivitätsstörung",</v>
+        <v>"child_list_item_7": "Eifersucht unter Geschwistern",</v>
       </c>
       <c r="G20" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B20,Sheet2!B$7,B20,Sheet2!B$8)</f>
-        <v>$("[data-lang=child_list_item_8]").text(language.child_list_item_8);</v>
+        <v>$("[data-lang=child_list_item_7]").text(language.child_list_item_7);</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E21" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B21,Sheet2!B$3,C21,Sheet2!B$4)</f>
-        <v>"child_list_item_9": "Okul ya da Akademik Konular İle İlgili Sorunlar",</v>
+        <v>"child_list_item_8": "Dikkat ve Hiperaktivite Bozukluğu",</v>
       </c>
       <c r="F21" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B21,Sheet2!B$3,D21,Sheet2!B$4)</f>
-        <v>"child_list_item_9": "Probleme im Zusammenhang mit schulischen oder akademischen Angelegenheiten",</v>
+        <v>"child_list_item_8": "Aufmerksamkeits- und Hyperaktivitätsstörung",</v>
       </c>
       <c r="G21" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B21,Sheet2!B$7,B21,Sheet2!B$8)</f>
-        <v>$("[data-lang=child_list_item_9]").text(language.child_list_item_9);</v>
+        <v>$("[data-lang=child_list_item_8]").text(language.child_list_item_8);</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E22" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B22,Sheet2!B$3,C22,Sheet2!B$4)</f>
-        <v>"child_list_item_10": "Öğrenme Güçlüğü",</v>
+        <v>"child_list_item_9": "Okul ya da Akademik Konular İle İlgili Sorunlar",</v>
       </c>
       <c r="F22" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B22,Sheet2!B$3,D22,Sheet2!B$4)</f>
-        <v>"child_list_item_10": "Lernschwierigkeiten",</v>
+        <v>"child_list_item_9": "Probleme im Zusammenhang mit schulischen oder akademischen Angelegenheiten",</v>
       </c>
       <c r="G22" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B22,Sheet2!B$7,B22,Sheet2!B$8)</f>
-        <v>$("[data-lang=child_list_item_10]").text(language.child_list_item_10);</v>
+        <v>$("[data-lang=child_list_item_9]").text(language.child_list_item_9);</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E23" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B23,Sheet2!B$3,C23,Sheet2!B$4)</f>
-        <v>"child_list_item_11": "Öfke ve Korkular",</v>
+        <v>"child_list_item_10": "Öğrenme Güçlüğü",</v>
       </c>
       <c r="F23" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B23,Sheet2!B$3,D23,Sheet2!B$4)</f>
-        <v>"child_list_item_11": "Wut und Ängste",</v>
+        <v>"child_list_item_10": "Lernschwierigkeiten",</v>
       </c>
       <c r="G23" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B23,Sheet2!B$7,B23,Sheet2!B$8)</f>
-        <v>$("[data-lang=child_list_item_11]").text(language.child_list_item_11);</v>
+        <v>$("[data-lang=child_list_item_10]").text(language.child_list_item_10);</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E24" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B24,Sheet2!B$3,C24,Sheet2!B$4)</f>
-        <v>"child_list_item_12": "Alt Islatma, Dışkı kaçırma, Tikler",</v>
+        <v>"child_list_item_11": "Öfke ve Korkular",</v>
       </c>
       <c r="F24" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B24,Sheet2!B$3,D24,Sheet2!B$4)</f>
-        <v>"child_list_item_12": "Bettnässen, Stuhlinkontinenz, Tics",</v>
+        <v>"child_list_item_11": "Wut und Ängste",</v>
       </c>
       <c r="G24" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B24,Sheet2!B$7,B24,Sheet2!B$8)</f>
-        <v>$("[data-lang=child_list_item_12]").text(language.child_list_item_12);</v>
+        <v>$("[data-lang=child_list_item_11]").text(language.child_list_item_11);</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E25" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B25,Sheet2!B$3,C25,Sheet2!B$4)</f>
-        <v>"child_list_item_13": "Travma, Kayıp, Yas Süreci",</v>
+        <v>"child_list_item_12": "Alt Islatma, Dışkı kaçırma, Tikler",</v>
       </c>
       <c r="F25" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B25,Sheet2!B$3,D25,Sheet2!B$4)</f>
-        <v>"child_list_item_13": "Trauma, Verlust, Trauerprozess",</v>
+        <v>"child_list_item_12": "Bettnässen, Stuhlinkontinenz, Tics",</v>
       </c>
       <c r="G25" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B25,Sheet2!B$7,B25,Sheet2!B$8)</f>
-        <v>$("[data-lang=child_list_item_13]").text(language.child_list_item_13);</v>
+        <v>$("[data-lang=child_list_item_12]").text(language.child_list_item_12);</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E26" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B26,Sheet2!B$3,C26,Sheet2!B$4)</f>
-        <v>"child_list_item_14": "Çocukluk Çağı Depresyon ve Kaygı Bozuklukları",</v>
+        <v>"child_list_item_13": "Travma, Kayıp, Yas Süreci",</v>
       </c>
       <c r="F26" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B26,Sheet2!B$3,D26,Sheet2!B$4)</f>
-        <v>"child_list_item_14": "Depressionen und Angstzustände in der Kindheit",</v>
+        <v>"child_list_item_13": "Trauma, Verlust, Trauerprozess",</v>
       </c>
       <c r="G26" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B26,Sheet2!B$7,B26,Sheet2!B$8)</f>
-        <v>$("[data-lang=child_list_item_14]").text(language.child_list_item_14);</v>
+        <v>$("[data-lang=child_list_item_13]").text(language.child_list_item_13);</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E27" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B27,Sheet2!B$3,C27,Sheet2!B$4)</f>
-        <v>"child_list_item_15": "Evlenme-Boşanmaya Bağlı Gelişen Sorunlar",</v>
+        <v>"child_list_item_14": "Çocukluk Çağı Depresyon ve Kaygı Bozuklukları",</v>
       </c>
       <c r="F27" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B27,Sheet2!B$3,D27,Sheet2!B$4)</f>
-        <v>"child_list_item_15": "Probleme im Zusammenhang mit Ehe und Scheidung",</v>
+        <v>"child_list_item_14": "Depressionen und Angstzustände in der Kindheit",</v>
       </c>
       <c r="G27" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B27,Sheet2!B$7,B27,Sheet2!B$8)</f>
-        <v>$("[data-lang=child_list_item_15]").text(language.child_list_item_15);</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>$("[data-lang=child_list_item_14]").text(language.child_list_item_14);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E28" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B28,Sheet2!B$3,C28,Sheet2!B$4)</f>
-        <v>"teenager_list_item_1": "Aileyle İlişki Sorunları",</v>
-      </c>
-      <c r="F28" t="str">
+        <v>"child_list_item_15": "Evlenme-Boşanmaya Bağlı Gelişen Sorunlar",</v>
+      </c>
+      <c r="F28" s="15" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B28,Sheet2!B$3,D28,Sheet2!B$4)</f>
-        <v>"teenager_list_item_1": "Beziehungsprobleme in der Familie",</v>
+        <v>"child_list_item_15": "Probleme im Zusammenhang mit Ehe und Scheidung",</v>
       </c>
       <c r="G28" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B28,Sheet2!B$7,B28,Sheet2!B$8)</f>
-        <v>$("[data-lang=teenager_list_item_1]").text(language.teenager_list_item_1);</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E29" t="str">
+        <v>$("[data-lang=child_list_item_15]").text(language.child_list_item_15);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="66" x14ac:dyDescent="0.25">
+      <c r="B29" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="E29" s="15" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B29,Sheet2!B$3,C29,Sheet2!B$4)</f>
-        <v>"teenager_list_item_2": "Uyum Sorunları",</v>
-      </c>
-      <c r="F29" t="str">
+        <v>"child_drawing_info_1": "3-11 yaş çocukları ile kendilerini daha iyi ifade edebilecekleri yöntemler kullanılarak iletişim kurmak gereklidir. Bu dönemde çocuğun iç dünyasının analiz edilmesi çizdiği resimler yoluyla kolayca mümkün olmaktadır. Bu çizimler sonucunda çocuğun ihtiyaçları belirlenebilmektedir.",</v>
+      </c>
+      <c r="F29" s="15" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B29,Sheet2!B$3,D29,Sheet2!B$4)</f>
-        <v>"teenager_list_item_2": "Anpassungsprobleme",</v>
-      </c>
-      <c r="G29" t="str">
+        <v>"child_drawing_info_1": "Es ist notwendig, mit Kindern im Alter von 3-11 Jahren zu kommunizieren, indem man Methoden verwendet, mit denen sie sich besser ausdrücken können.
+In dieser Zeit ist die Analyse der inneren Welt des Kindes anhand der Zeichnungen leicht möglich. Anhand dieser Zeichnungen lassen sich die Bedürfnisse des Kindes ermitteln.",</v>
+      </c>
+      <c r="G29" s="10" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B29,Sheet2!B$7,B29,Sheet2!B$8)</f>
-        <v>$("[data-lang=teenager_list_item_2]").text(language.teenager_list_item_2);</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="8" t="s">
-        <v>144</v>
+        <v>$("[data-lang=child_drawing_info_1]").text(language.child_drawing_info_1);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>182</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>38</v>
+        <v>176</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>14</v>
+        <v>175</v>
       </c>
       <c r="E30" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B30,Sheet2!B$3,C30,Sheet2!B$4)</f>
-        <v>"teenager_list_item_3": "Arkadaş İlişkileri İle İlgili sorunlar",</v>
+        <v>"teenager_section_sub_title": "Ergen Terapisi",</v>
       </c>
       <c r="F30" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B30,Sheet2!B$3,D30,Sheet2!B$4)</f>
-        <v>"teenager_list_item_3": "Probleme mit Freundschaftsbeziehungen",</v>
+        <v>"teenager_section_sub_title": "Jugendliche Therapy",</v>
       </c>
       <c r="G30" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B30,Sheet2!B$7,B30,Sheet2!B$8)</f>
-        <v>$("[data-lang=teenager_list_item_3]").text(language.teenager_list_item_3);</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>$("[data-lang=teenager_section_sub_title]").text(language.teenager_section_sub_title);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E31" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B31,Sheet2!B$3,C31,Sheet2!B$4)</f>
-        <v>"teenager_list_item_4": "Karşı Cinsle İlgili Konular",</v>
+        <v>"teenager_list_item_1": "Aileyle İlişki Sorunları",</v>
       </c>
       <c r="F31" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B31,Sheet2!B$3,D31,Sheet2!B$4)</f>
-        <v>"teenager_list_item_4": "Themen im Zusammenhang mit dem anderen Geschlecht",</v>
+        <v>"teenager_list_item_1": "Beziehungsprobleme in der Familie",</v>
       </c>
       <c r="G31" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B31,Sheet2!B$7,B31,Sheet2!B$8)</f>
-        <v>$("[data-lang=teenager_list_item_4]").text(language.teenager_list_item_4);</v>
+        <v>$("[data-lang=teenager_list_item_1]").text(language.teenager_list_item_1);</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>41</v>
+        <v>143</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E32" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B32,Sheet2!B$3,C32,Sheet2!B$4)</f>
-        <v>"teenager_list_item_5": "Okul ve Akademik Konular İle İlgili Sorunlar",</v>
+        <v>"teenager_list_item_2": "Uyum Sorunları",</v>
       </c>
       <c r="F32" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B32,Sheet2!B$3,D32,Sheet2!B$4)</f>
-        <v>"teenager_list_item_5": "Probleme im Zusammenhang mit schulischen und akademischen Fragen",</v>
+        <v>"teenager_list_item_2": "Anpassungsprobleme",</v>
       </c>
       <c r="G32" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B32,Sheet2!B$7,B32,Sheet2!B$8)</f>
-        <v>$("[data-lang=teenager_list_item_5]").text(language.teenager_list_item_5);</v>
+        <v>$("[data-lang=teenager_list_item_2]").text(language.teenager_list_item_2);</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="E33" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B33,Sheet2!B$3,C33,Sheet2!B$4)</f>
-        <v>"teenager_list_item_6": "Kaygı, Korku ve Öfke Sorunları",</v>
+        <v>"teenager_list_item_3": "Arkadaş İlişkileri İle İlgili sorunlar",</v>
       </c>
       <c r="F33" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B33,Sheet2!B$3,D33,Sheet2!B$4)</f>
-        <v>"teenager_list_item_6": "Probleme mit Ängsten, Furcht und Wut",</v>
+        <v>"teenager_list_item_3": "Probleme mit Freundschaftsbeziehungen",</v>
       </c>
       <c r="G33" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B33,Sheet2!B$7,B33,Sheet2!B$8)</f>
-        <v>$("[data-lang=teenager_list_item_6]").text(language.teenager_list_item_6);</v>
+        <v>$("[data-lang=teenager_list_item_3]").text(language.teenager_list_item_3);</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>45</v>
+        <v>145</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E34" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B34,Sheet2!B$3,C34,Sheet2!B$4)</f>
-        <v>"teenager_list_item_7": "Ergenlik ve Gelişim İle İlgili Sorunlar",</v>
+        <v>"teenager_list_item_4": "Karşı Cinsle İlgili Konular",</v>
       </c>
       <c r="F34" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B34,Sheet2!B$3,D34,Sheet2!B$4)</f>
-        <v>"teenager_list_item_7": "Probleme im Zusammenhang mit der Adoleszenz und der Entwicklung",</v>
+        <v>"teenager_list_item_4": "Themen im Zusammenhang mit dem anderen Geschlecht",</v>
       </c>
       <c r="G34" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B34,Sheet2!B$7,B34,Sheet2!B$8)</f>
-        <v>$("[data-lang=teenager_list_item_7]").text(language.teenager_list_item_7);</v>
+        <v>$("[data-lang=teenager_list_item_4]").text(language.teenager_list_item_4);</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>47</v>
+        <v>146</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E35" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B35,Sheet2!B$3,C35,Sheet2!B$4)</f>
-        <v>"teenager_list_item_8": "Travma, Depresyon ve Kimlik Bunalımı",</v>
+        <v>"teenager_list_item_5": "Okul ve Akademik Konular İle İlgili Sorunlar",</v>
       </c>
       <c r="F35" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B35,Sheet2!B$3,D35,Sheet2!B$4)</f>
-        <v>"teenager_list_item_8": "Trauma, Depressionen und Identitätskrisen",</v>
+        <v>"teenager_list_item_5": "Probleme im Zusammenhang mit schulischen und akademischen Fragen",</v>
       </c>
       <c r="G35" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B35,Sheet2!B$7,B35,Sheet2!B$8)</f>
-        <v>$("[data-lang=teenager_list_item_8]").text(language.teenager_list_item_8);</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>49</v>
+        <v>$("[data-lang=teenager_list_item_5]").text(language.teenager_list_item_5);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B36" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E36" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B36,Sheet2!B$3,C36,Sheet2!B$4)</f>
-        <v>"teenager_list_item_9": "Özgüven Kaybı İle İlgili Sorunlar",</v>
+        <v>"teenager_list_item_6": "Kaygı, Korku ve Öfke Sorunları",</v>
       </c>
       <c r="F36" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B36,Sheet2!B$3,D36,Sheet2!B$4)</f>
-        <v>"teenager_list_item_9": "Probleme im Zusammenhang mit dem Verlust des Selbstbewusstseins",</v>
+        <v>"teenager_list_item_6": "Probleme mit Ängsten, Furcht und Wut",</v>
       </c>
       <c r="G36" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B36,Sheet2!B$7,B36,Sheet2!B$8)</f>
-        <v>$("[data-lang=teenager_list_item_9]").text(language.teenager_list_item_9);</v>
+        <v>$("[data-lang=teenager_list_item_6]").text(language.teenager_list_item_6);</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E37" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B37,Sheet2!B$3,C37,Sheet2!B$4)</f>
-        <v>"teenager_list_item_10": "Bağımlılık",</v>
+        <v>"teenager_list_item_7": "Ergenlik ve Gelişim İle İlgili Sorunlar",</v>
       </c>
       <c r="F37" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B37,Sheet2!B$3,D37,Sheet2!B$4)</f>
-        <v>"teenager_list_item_10": "Sucht",</v>
+        <v>"teenager_list_item_7": "Probleme im Zusammenhang mit der Adoleszenz und der Entwicklung",</v>
       </c>
       <c r="G37" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B37,Sheet2!B$7,B37,Sheet2!B$8)</f>
-        <v>$("[data-lang=teenager_list_item_10]").text(language.teenager_list_item_10);</v>
+        <v>$("[data-lang=teenager_list_item_7]").text(language.teenager_list_item_7);</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="B38" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E38" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B38,Sheet2!B$3,C38,Sheet2!B$4)</f>
-        <v>"adult_list_item_1": "Depresyon",</v>
+        <v>"teenager_list_item_8": "Travma, Depresyon ve Kimlik Bunalımı",</v>
       </c>
       <c r="F38" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B38,Sheet2!B$3,D38,Sheet2!B$4)</f>
-        <v>"adult_list_item_1": "Depression",</v>
+        <v>"teenager_list_item_8": "Trauma, Depressionen und Identitätskrisen",</v>
       </c>
       <c r="G38" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B38,Sheet2!B$7,B38,Sheet2!B$8)</f>
-        <v>$("[data-lang=adult_list_item_1]").text(language.adult_list_item_1);</v>
+        <v>$("[data-lang=teenager_list_item_8]").text(language.teenager_list_item_8);</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>56</v>
+        <v>150</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E39" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B39,Sheet2!B$3,C39,Sheet2!B$4)</f>
-        <v>"adult_list_item_2": "Kaygı Bozuklukları",</v>
+        <v>"teenager_list_item_9": "Özgüven Kaybı İle İlgili Sorunlar",</v>
       </c>
       <c r="F39" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B39,Sheet2!B$3,D39,Sheet2!B$4)</f>
-        <v>"adult_list_item_2": "Angst-Störungen",</v>
+        <v>"teenager_list_item_9": "Probleme im Zusammenhang mit dem Verlust des Selbstbewusstseins",</v>
       </c>
       <c r="G39" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B39,Sheet2!B$7,B39,Sheet2!B$8)</f>
-        <v>$("[data-lang=adult_list_item_2]").text(language.adult_list_item_2);</v>
+        <v>$("[data-lang=teenager_list_item_9]").text(language.teenager_list_item_9);</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>58</v>
+        <v>151</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E40" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B40,Sheet2!B$3,C40,Sheet2!B$4)</f>
-        <v>"adult_list_item_3": "Panik Atak",</v>
+        <v>"teenager_list_item_10": "Bağımlılık",</v>
       </c>
       <c r="F40" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B40,Sheet2!B$3,D40,Sheet2!B$4)</f>
-        <v>"adult_list_item_3": "Panikattacke",</v>
+        <v>"teenager_list_item_10": "Sucht",</v>
       </c>
       <c r="G40" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B40,Sheet2!B$7,B40,Sheet2!B$8)</f>
-        <v>$("[data-lang=adult_list_item_3]").text(language.adult_list_item_3);</v>
+        <v>$("[data-lang=teenager_list_item_10]").text(language.teenager_list_item_10);</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="B41" s="8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E41" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B41,Sheet2!B$3,C41,Sheet2!B$4)</f>
-        <v>"adult_list_item_4": "Sosyal Fobi",</v>
+        <v>"adult_list_item_1": "Depresyon",</v>
       </c>
       <c r="F41" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B41,Sheet2!B$3,D41,Sheet2!B$4)</f>
-        <v>"adult_list_item_4": "Sozialphobie",</v>
+        <v>"adult_list_item_1": "Depression",</v>
       </c>
       <c r="G41" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B41,Sheet2!B$7,B41,Sheet2!B$8)</f>
-        <v>$("[data-lang=adult_list_item_4]").text(language.adult_list_item_4);</v>
+        <v>$("[data-lang=adult_list_item_1]").text(language.adult_list_item_1);</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E42" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B42,Sheet2!B$3,C42,Sheet2!B$4)</f>
-        <v>"adult_list_item_5": "İlişki Sorunları",</v>
+        <v>"adult_list_item_2": "Kaygı Bozuklukları",</v>
       </c>
       <c r="F42" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B42,Sheet2!B$3,D42,Sheet2!B$4)</f>
-        <v>"adult_list_item_5": "Beziehungsprobleme",</v>
+        <v>"adult_list_item_2": "Angst-Störungen",</v>
       </c>
       <c r="G42" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B42,Sheet2!B$7,B42,Sheet2!B$8)</f>
-        <v>$("[data-lang=adult_list_item_5]").text(language.adult_list_item_5);</v>
+        <v>$("[data-lang=adult_list_item_2]").text(language.adult_list_item_2);</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E43" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B43,Sheet2!B$3,C43,Sheet2!B$4)</f>
-        <v>"adult_list_item_6": "Uyku Bozuklukları",</v>
+        <v>"adult_list_item_3": "Panik Atak",</v>
       </c>
       <c r="F43" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B43,Sheet2!B$3,D43,Sheet2!B$4)</f>
-        <v>"adult_list_item_6": "Schlafstörungen",</v>
+        <v>"adult_list_item_3": "Panikattacke",</v>
       </c>
       <c r="G43" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B43,Sheet2!B$7,B43,Sheet2!B$8)</f>
-        <v>$("[data-lang=adult_list_item_6]").text(language.adult_list_item_6);</v>
+        <v>$("[data-lang=adult_list_item_3]").text(language.adult_list_item_3);</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E44" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B44,Sheet2!B$3,C44,Sheet2!B$4)</f>
-        <v>"adult_list_item_7": "Yeme Bozuklukları",</v>
+        <v>"adult_list_item_4": "Sosyal Fobi",</v>
       </c>
       <c r="F44" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B44,Sheet2!B$3,D44,Sheet2!B$4)</f>
-        <v>"adult_list_item_7": "Ess-Störungen",</v>
+        <v>"adult_list_item_4": "Sozialphobie",</v>
       </c>
       <c r="G44" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B44,Sheet2!B$7,B44,Sheet2!B$8)</f>
-        <v>$("[data-lang=adult_list_item_7]").text(language.adult_list_item_7);</v>
+        <v>$("[data-lang=adult_list_item_4]").text(language.adult_list_item_4);</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" s="8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E45" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B45,Sheet2!B$3,C45,Sheet2!B$4)</f>
-        <v>"adult_list_item_8": "Öfke Problemleri",</v>
+        <v>"adult_list_item_5": "İlişki Sorunları",</v>
       </c>
       <c r="F45" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B45,Sheet2!B$3,D45,Sheet2!B$4)</f>
-        <v>"adult_list_item_8": "Probleme mit Wut",</v>
+        <v>"adult_list_item_5": "Beziehungsprobleme",</v>
       </c>
       <c r="G45" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B45,Sheet2!B$7,B45,Sheet2!B$8)</f>
-        <v>$("[data-lang=adult_list_item_8]").text(language.adult_list_item_8);</v>
+        <v>$("[data-lang=adult_list_item_5]").text(language.adult_list_item_5);</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B46" s="8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E46" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B46,Sheet2!B$3,C46,Sheet2!B$4)</f>
-        <v>"adult_list_item_9": "Obsesif Kompulsif Bozukluk",</v>
+        <v>"adult_list_item_6": "Uyku Bozuklukları",</v>
       </c>
       <c r="F46" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B46,Sheet2!B$3,D46,Sheet2!B$4)</f>
-        <v>"adult_list_item_9": "Zwangsneurose",</v>
+        <v>"adult_list_item_6": "Schlafstörungen",</v>
       </c>
       <c r="G46" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B46,Sheet2!B$7,B46,Sheet2!B$8)</f>
-        <v>$("[data-lang=adult_list_item_9]").text(language.adult_list_item_9);</v>
+        <v>$("[data-lang=adult_list_item_6]").text(language.adult_list_item_6);</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" s="8" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E47" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B47,Sheet2!B$3,C47,Sheet2!B$4)</f>
-        <v>"adult_list_item_10": "Travma ve Stres Bağlantılı Bozukluk",</v>
+        <v>"adult_list_item_7": "Yeme Bozuklukları",</v>
       </c>
       <c r="F47" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B47,Sheet2!B$3,D47,Sheet2!B$4)</f>
-        <v>"adult_list_item_10": "Trauma und stressbedingte Störungen",</v>
+        <v>"adult_list_item_7": "Ess-Störungen",</v>
       </c>
       <c r="G47" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B47,Sheet2!B$7,B47,Sheet2!B$8)</f>
-        <v>$("[data-lang=adult_list_item_10]").text(language.adult_list_item_10);</v>
+        <v>$("[data-lang=adult_list_item_7]").text(language.adult_list_item_7);</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E48" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B48,Sheet2!B$3,C48,Sheet2!B$4)</f>
-        <v>"adult_list_item_11": "Psikosomatik Bozukluklar",</v>
+        <v>"adult_list_item_8": "Öfke Problemleri",</v>
       </c>
       <c r="F48" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B48,Sheet2!B$3,D48,Sheet2!B$4)</f>
-        <v>"adult_list_item_11": "Psychosomatische Störungen",</v>
+        <v>"adult_list_item_8": "Probleme mit Wut",</v>
       </c>
       <c r="G48" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B48,Sheet2!B$7,B48,Sheet2!B$8)</f>
-        <v>$("[data-lang=adult_list_item_11]").text(language.adult_list_item_11);</v>
+        <v>$("[data-lang=adult_list_item_8]").text(language.adult_list_item_8);</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B49" s="8" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E49" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B49,Sheet2!B$3,C49,Sheet2!B$4)</f>
-        <v>"adult_list_item_12": "Psikotik Bozukluklar",</v>
+        <v>"adult_list_item_9": "Obsesif Kompulsif Bozukluk",</v>
       </c>
       <c r="F49" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B49,Sheet2!B$3,D49,Sheet2!B$4)</f>
-        <v>"adult_list_item_12": "Psychotische Störungen",</v>
+        <v>"adult_list_item_9": "Zwangsneurose",</v>
       </c>
       <c r="G49" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B49,Sheet2!B$7,B49,Sheet2!B$8)</f>
-        <v>$("[data-lang=adult_list_item_12]").text(language.adult_list_item_12);</v>
+        <v>$("[data-lang=adult_list_item_9]").text(language.adult_list_item_9);</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B50" s="8" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E50" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B50,Sheet2!B$3,C50,Sheet2!B$4)</f>
-        <v>"adult_list_item_13": "İş-Özel Yaşam Dengesi ve Sosyal Sorunlar",</v>
+        <v>"adult_list_item_10": "Travma ve Stres Bağlantılı Bozukluk",</v>
       </c>
       <c r="F50" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B50,Sheet2!B$3,D50,Sheet2!B$4)</f>
-        <v>"adult_list_item_13": "Work-Life-Balance und soziale Probleme",</v>
+        <v>"adult_list_item_10": "Trauma und stressbedingte Störungen",</v>
       </c>
       <c r="G50" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B50,Sheet2!B$7,B50,Sheet2!B$8)</f>
-        <v>$("[data-lang=adult_list_item_13]").text(language.adult_list_item_13);</v>
+        <v>$("[data-lang=adult_list_item_10]").text(language.adult_list_item_10);</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B51" s="8" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E51" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B51,Sheet2!B$3,C51,Sheet2!B$4)</f>
-        <v>"adult_list_item_14": "Duygu ve Duygulanım Sorunları, Mutsuzluk",</v>
+        <v>"adult_list_item_11": "Psikosomatik Bozukluklar",</v>
       </c>
       <c r="F51" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B51,Sheet2!B$3,D51,Sheet2!B$4)</f>
-        <v>"adult_list_item_14": "Emotionale und affektive Probleme, Unglücklichsein",</v>
+        <v>"adult_list_item_11": "Psychosomatische Störungen",</v>
       </c>
       <c r="G51" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B51,Sheet2!B$7,B51,Sheet2!B$8)</f>
-        <v>$("[data-lang=adult_list_item_14]").text(language.adult_list_item_14);</v>
+        <v>$("[data-lang=adult_list_item_11]").text(language.adult_list_item_11);</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="B52" s="8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E52" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B52,Sheet2!B$3,C52,Sheet2!B$4)</f>
-        <v>"family_list_item_1": "Aile İçerisinde İlişki ve İletişim Sorunları",</v>
+        <v>"adult_list_item_12": "Psikotik Bozukluklar",</v>
       </c>
       <c r="F52" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B52,Sheet2!B$3,D52,Sheet2!B$4)</f>
-        <v>"family_list_item_1": "Beziehungs- und Kommunikationsprobleme in der Familie",</v>
+        <v>"adult_list_item_12": "Psychotische Störungen",</v>
       </c>
       <c r="G52" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B52,Sheet2!B$7,B52,Sheet2!B$8)</f>
-        <v>$("[data-lang=family_list_item_1]").text(language.family_list_item_1);</v>
+        <v>$("[data-lang=adult_list_item_12]").text(language.adult_list_item_12);</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B53" s="8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E53" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B53,Sheet2!B$3,C53,Sheet2!B$4)</f>
-        <v>"family_list_item_2": "Sosyal İlişkilerde Yaşanan Sorunlar",</v>
+        <v>"adult_list_item_13": "İş-Özel Yaşam Dengesi ve Sosyal Sorunlar",</v>
       </c>
       <c r="F53" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B53,Sheet2!B$3,D53,Sheet2!B$4)</f>
-        <v>"family_list_item_2": "Probleme in sozialen Beziehungen",</v>
+        <v>"adult_list_item_13": "Work-Life-Balance und soziale Probleme",</v>
       </c>
       <c r="G53" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B53,Sheet2!B$7,B53,Sheet2!B$8)</f>
-        <v>$("[data-lang=family_list_item_2]").text(language.family_list_item_2);</v>
+        <v>$("[data-lang=adult_list_item_13]").text(language.adult_list_item_13);</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="9" t="s">
-        <v>168</v>
+      <c r="B54" s="8" t="s">
+        <v>165</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E54" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B54,Sheet2!B$3,C54,Sheet2!B$4)</f>
-        <v>"family_list_item_3": "Nişanlılık, Evlilik ve Boşanma Konuları İle İlgili Sorunlar",</v>
+        <v>"adult_list_item_14": "Duygu ve Duygulanım Sorunları, Mutsuzluk",</v>
       </c>
       <c r="F54" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$2, B54,Sheet2!B$3,D54,Sheet2!B$4)</f>
-        <v>"family_list_item_3": "Probleme im Zusammenhang mit Verlobung, Heirat und Scheidung",</v>
+        <v>"adult_list_item_14": "Emotionale und affektive Probleme, Unglücklichsein",</v>
       </c>
       <c r="G54" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B54,Sheet2!B$7,B54,Sheet2!B$8)</f>
+        <v>$("[data-lang=adult_list_item_14]").text(language.adult_list_item_14);</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E55" t="str">
+        <f>_xlfn.CONCAT(Sheet2!B$2, B55,Sheet2!B$3,C55,Sheet2!B$4)</f>
+        <v>"family_list_item_1": "Aile İçerisinde İlişki ve İletişim Sorunları",</v>
+      </c>
+      <c r="F55" t="str">
+        <f>_xlfn.CONCAT(Sheet2!B$2, B55,Sheet2!B$3,D55,Sheet2!B$4)</f>
+        <v>"family_list_item_1": "Beziehungs- und Kommunikationsprobleme in der Familie",</v>
+      </c>
+      <c r="G55" t="str">
+        <f>_xlfn.CONCAT(Sheet2!B$6,B55,Sheet2!B$7,B55,Sheet2!B$8)</f>
+        <v>$("[data-lang=family_list_item_1]").text(language.family_list_item_1);</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E56" t="str">
+        <f>_xlfn.CONCAT(Sheet2!B$2, B56,Sheet2!B$3,C56,Sheet2!B$4)</f>
+        <v>"family_list_item_2": "Sosyal İlişkilerde Yaşanan Sorunlar",</v>
+      </c>
+      <c r="F56" t="str">
+        <f>_xlfn.CONCAT(Sheet2!B$2, B56,Sheet2!B$3,D56,Sheet2!B$4)</f>
+        <v>"family_list_item_2": "Probleme in sozialen Beziehungen",</v>
+      </c>
+      <c r="G56" t="str">
+        <f>_xlfn.CONCAT(Sheet2!B$6,B56,Sheet2!B$7,B56,Sheet2!B$8)</f>
+        <v>$("[data-lang=family_list_item_2]").text(language.family_list_item_2);</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E57" t="str">
+        <f>_xlfn.CONCAT(Sheet2!B$2, B57,Sheet2!B$3,C57,Sheet2!B$4)</f>
+        <v>"family_list_item_3": "Nişanlılık, Evlilik ve Boşanma Konuları İle İlgili Sorunlar",</v>
+      </c>
+      <c r="F57" t="str">
+        <f>_xlfn.CONCAT(Sheet2!B$2, B57,Sheet2!B$3,D57,Sheet2!B$4)</f>
+        <v>"family_list_item_3": "Probleme im Zusammenhang mit Verlobung, Heirat und Scheidung",</v>
+      </c>
+      <c r="G57" t="str">
+        <f>_xlfn.CONCAT(Sheet2!B$6,B57,Sheet2!B$7,B57,Sheet2!B$8)</f>
         <v>$("[data-lang=family_list_item_3]").text(language.family_list_item_3);</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="D58" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="E58" s="15" t="str">
+        <f>_xlfn.CONCAT(Sheet2!B$2, B58,Sheet2!B$3,C58,Sheet2!B$4)</f>
+        <v>"game_therapy_info_1": "Oyun; çocuğun kendini ifade etmesi, hayal ile gerçek arasında bir köprü, gizli enerjinin kullanılması, çocuğun sosyal ve ahlaki değerleri öğrendiği bir alandır.",</v>
+      </c>
+      <c r="F58" s="15" t="str">
+        <f>_xlfn.CONCAT(Sheet2!B$2, B58,Sheet2!B$3,D58,Sheet2!B$4)</f>
+        <v>"game_therapy_info_1": "Spiel; ist ein Bereich, in dem das Kind sich selbst ausdrückt, eine Brücke zwischen Phantasie und Realität, die Nutzung verborgener Energien, und in dem das Kind soziale und moralische Werte erlernt.",</v>
+      </c>
+      <c r="G58" s="10" t="str">
+        <f>_xlfn.CONCAT(Sheet2!B$6,B58,Sheet2!B$7,B58,Sheet2!B$8)</f>
+        <v>$("[data-lang=game_therapy_info_1]").text(language.game_therapy_info_1);</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add new text resources
</commit_message>
<xml_diff>
--- a/TherapyHessen/doc/Translation-Therapy-Hessen.xlsx
+++ b/TherapyHessen/doc/Translation-Therapy-Hessen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Trunk\Samples\TherapyHessen\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5BE5C6-08C9-4CD1-899C-BAFC7B651DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A8C636-316A-4347-B5D5-DAC5CFAF014E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1440" windowWidth="38640" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="189">
   <si>
     <t>Turkish</t>
   </si>
@@ -589,6 +588,18 @@
   </si>
   <si>
     <t>child_section_sub_title</t>
+  </si>
+  <si>
+    <t>Karsilama Metni</t>
+  </si>
+  <si>
+    <t>Ben bir Psikolog olarak dünyaya gelmedim. insan olarak varlığımı ve onun anlamını keşfetmeye geldim. Bu keşif yolculuğum ise beni bu değerli meslekle buluşturdu. şimdi her şey çok daha anlamlı. Çünkü; yolculuğumda ben insanların hayatına dokunmaya başladım ve bu çok özel.</t>
+  </si>
+  <si>
+    <t>Ich wurde nicht als Psychologe geboren. Ich habe meine Existenz als Mensch und deren Bedeutung entdeckt. Diese Entdeckungsreise hat mich mit diesem wertvollen Beruf zusammengebracht. Jetzt ist alles viel sinnvoller. Denn auf meiner Reise habe ich begonnen, das Leben von Menschen zu berühren, und das ist etwas ganz Besonderes.</t>
+  </si>
+  <si>
+    <t>home_greeting_text</t>
   </si>
 </sst>
 </file>
@@ -712,7 +723,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -743,6 +754,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -961,10 +973,12 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -978,7 +992,7 @@
     <col min="7" max="7" width="87.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="11" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
@@ -995,7 +1009,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>94</v>
       </c>
@@ -1018,7 +1032,7 @@
         <v>$("[data-lang=date]").text(language.date);</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>117</v>
       </c>
@@ -1041,7 +1055,7 @@
         <v>$("[data-lang=navigation_text_1]").text(language.navigation_text_1);</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>118</v>
       </c>
@@ -1064,7 +1078,7 @@
         <v>$("[data-lang=navigation_text_2]").text(language.navigation_text_2);</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
         <v>119</v>
       </c>
@@ -1087,7 +1101,7 @@
         <v>$("[data-lang=navigation_text_3]").text(language.navigation_text_3);</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>120</v>
       </c>
@@ -1110,7 +1124,7 @@
         <v>$("[data-lang=navigation_text_4]").text(language.navigation_text_4);</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>121</v>
       </c>
@@ -1133,7 +1147,7 @@
         <v>$("[data-lang=navigation_text_5]").text(language.navigation_text_5);</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>122</v>
       </c>
@@ -1156,7 +1170,7 @@
         <v>$("[data-lang=navigation_text_6]").text(language.navigation_text_6);</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>123</v>
       </c>
@@ -1179,7 +1193,7 @@
         <v>$("[data-lang=job_title]").text(language.job_title);</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>124</v>
       </c>
@@ -1202,7 +1216,7 @@
         <v>$("[data-lang=job_short_description]").text(language.job_short_description);</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>125</v>
       </c>
@@ -1225,7 +1239,7 @@
         <v>$("[data-lang=welcome_title]").text(language.welcome_title);</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>126</v>
       </c>
@@ -1274,7 +1288,7 @@
         <v>$("[data-lang=child_section_sub_title]").text(language.child_section_sub_title);</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="8" t="s">
         <v>127</v>
@@ -1298,7 +1312,7 @@
         <v>$("[data-lang=child_list_item_1]").text(language.child_list_item_1);</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>128</v>
       </c>
@@ -1321,7 +1335,7 @@
         <v>$("[data-lang=child_list_item_2]").text(language.child_list_item_2);</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>129</v>
       </c>
@@ -1344,7 +1358,7 @@
         <v>$("[data-lang=child_list_item_3]").text(language.child_list_item_3);</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>130</v>
       </c>
@@ -1367,7 +1381,7 @@
         <v>$("[data-lang=child_list_item_4]").text(language.child_list_item_4);</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>131</v>
       </c>
@@ -1390,7 +1404,7 @@
         <v>$("[data-lang=child_list_item_5]").text(language.child_list_item_5);</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>132</v>
       </c>
@@ -1413,7 +1427,7 @@
         <v>$("[data-lang=child_list_item_6]").text(language.child_list_item_6);</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
         <v>133</v>
       </c>
@@ -1436,7 +1450,7 @@
         <v>$("[data-lang=child_list_item_7]").text(language.child_list_item_7);</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
         <v>134</v>
       </c>
@@ -1459,7 +1473,7 @@
         <v>$("[data-lang=child_list_item_8]").text(language.child_list_item_8);</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
         <v>135</v>
       </c>
@@ -1482,7 +1496,7 @@
         <v>$("[data-lang=child_list_item_9]").text(language.child_list_item_9);</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
         <v>136</v>
       </c>
@@ -1505,7 +1519,7 @@
         <v>$("[data-lang=child_list_item_10]").text(language.child_list_item_10);</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
         <v>137</v>
       </c>
@@ -1528,7 +1542,7 @@
         <v>$("[data-lang=child_list_item_11]").text(language.child_list_item_11);</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>138</v>
       </c>
@@ -1551,7 +1565,7 @@
         <v>$("[data-lang=child_list_item_12]").text(language.child_list_item_12);</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
         <v>139</v>
       </c>
@@ -1574,7 +1588,7 @@
         <v>$("[data-lang=child_list_item_13]").text(language.child_list_item_13);</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
         <v>140</v>
       </c>
@@ -1693,7 +1707,7 @@
         <v>$("[data-lang=teenager_list_item_1]").text(language.teenager_list_item_1);</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
         <v>143</v>
       </c>
@@ -1716,7 +1730,7 @@
         <v>$("[data-lang=teenager_list_item_2]").text(language.teenager_list_item_2);</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>144</v>
       </c>
@@ -1739,7 +1753,7 @@
         <v>$("[data-lang=teenager_list_item_3]").text(language.teenager_list_item_3);</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>145</v>
       </c>
@@ -1762,7 +1776,7 @@
         <v>$("[data-lang=teenager_list_item_4]").text(language.teenager_list_item_4);</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>146</v>
       </c>
@@ -1808,7 +1822,7 @@
         <v>$("[data-lang=teenager_list_item_6]").text(language.teenager_list_item_6);</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
         <v>148</v>
       </c>
@@ -1831,7 +1845,7 @@
         <v>$("[data-lang=teenager_list_item_7]").text(language.teenager_list_item_7);</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>149</v>
       </c>
@@ -1854,7 +1868,7 @@
         <v>$("[data-lang=teenager_list_item_8]").text(language.teenager_list_item_8);</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B39" s="8" t="s">
         <v>150</v>
       </c>
@@ -1877,7 +1891,7 @@
         <v>$("[data-lang=teenager_list_item_9]").text(language.teenager_list_item_9);</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B40" s="8" t="s">
         <v>151</v>
       </c>
@@ -1900,7 +1914,7 @@
         <v>$("[data-lang=teenager_list_item_10]").text(language.teenager_list_item_10);</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>53</v>
       </c>
@@ -1926,7 +1940,7 @@
         <v>$("[data-lang=adult_list_item_1]").text(language.adult_list_item_1);</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B42" s="8" t="s">
         <v>153</v>
       </c>
@@ -1949,7 +1963,7 @@
         <v>$("[data-lang=adult_list_item_2]").text(language.adult_list_item_2);</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="8" t="s">
         <v>154</v>
       </c>
@@ -1972,7 +1986,7 @@
         <v>$("[data-lang=adult_list_item_3]").text(language.adult_list_item_3);</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B44" s="8" t="s">
         <v>155</v>
       </c>
@@ -1995,7 +2009,7 @@
         <v>$("[data-lang=adult_list_item_4]").text(language.adult_list_item_4);</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B45" s="8" t="s">
         <v>156</v>
       </c>
@@ -2018,7 +2032,7 @@
         <v>$("[data-lang=adult_list_item_5]").text(language.adult_list_item_5);</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B46" s="8" t="s">
         <v>157</v>
       </c>
@@ -2041,7 +2055,7 @@
         <v>$("[data-lang=adult_list_item_6]").text(language.adult_list_item_6);</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B47" s="8" t="s">
         <v>158</v>
       </c>
@@ -2064,7 +2078,7 @@
         <v>$("[data-lang=adult_list_item_7]").text(language.adult_list_item_7);</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
         <v>159</v>
       </c>
@@ -2087,7 +2101,7 @@
         <v>$("[data-lang=adult_list_item_8]").text(language.adult_list_item_8);</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B49" s="8" t="s">
         <v>160</v>
       </c>
@@ -2110,7 +2124,7 @@
         <v>$("[data-lang=adult_list_item_9]").text(language.adult_list_item_9);</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B50" s="8" t="s">
         <v>161</v>
       </c>
@@ -2133,7 +2147,7 @@
         <v>$("[data-lang=adult_list_item_10]").text(language.adult_list_item_10);</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B51" s="8" t="s">
         <v>162</v>
       </c>
@@ -2156,7 +2170,7 @@
         <v>$("[data-lang=adult_list_item_11]").text(language.adult_list_item_11);</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B52" s="8" t="s">
         <v>163</v>
       </c>
@@ -2179,7 +2193,7 @@
         <v>$("[data-lang=adult_list_item_12]").text(language.adult_list_item_12);</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B53" s="8" t="s">
         <v>164</v>
       </c>
@@ -2202,7 +2216,7 @@
         <v>$("[data-lang=adult_list_item_13]").text(language.adult_list_item_13);</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B54" s="8" t="s">
         <v>165</v>
       </c>
@@ -2225,7 +2239,7 @@
         <v>$("[data-lang=adult_list_item_14]").text(language.adult_list_item_14);</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>82</v>
       </c>
@@ -2251,7 +2265,7 @@
         <v>$("[data-lang=family_list_item_1]").text(language.family_list_item_1);</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B56" s="8" t="s">
         <v>167</v>
       </c>
@@ -2274,7 +2288,7 @@
         <v>$("[data-lang=family_list_item_2]").text(language.family_list_item_2);</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B57" s="9" t="s">
         <v>168</v>
       </c>
@@ -2318,6 +2332,32 @@
       <c r="G58" s="10" t="str">
         <f>_xlfn.CONCAT(Sheet2!B$6,B58,Sheet2!B$7,B58,Sheet2!B$8)</f>
         <v>$("[data-lang=game_therapy_info_1]").text(language.game_therapy_info_1);</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>185</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="E59" s="15" t="str">
+        <f>_xlfn.CONCAT(Sheet2!B$2, B59,Sheet2!B$3,C59,Sheet2!B$4)</f>
+        <v>"home_greeting_text": "Ben bir Psikolog olarak dünyaya gelmedim. insan olarak varlığımı ve onun anlamını keşfetmeye geldim. Bu keşif yolculuğum ise beni bu değerli meslekle buluşturdu. şimdi her şey çok daha anlamlı. Çünkü; yolculuğumda ben insanların hayatına dokunmaya başladım ve bu çok özel.",</v>
+      </c>
+      <c r="F59" s="15" t="str">
+        <f>_xlfn.CONCAT(Sheet2!B$2, B59,Sheet2!B$3,D59,Sheet2!B$4)</f>
+        <v>"home_greeting_text": "Ich wurde nicht als Psychologe geboren. Ich habe meine Existenz als Mensch und deren Bedeutung entdeckt. Diese Entdeckungsreise hat mich mit diesem wertvollen Beruf zusammengebracht. Jetzt ist alles viel sinnvoller. Denn auf meiner Reise habe ich begonnen, das Leben von Menschen zu berühren, und das ist etwas ganz Besonderes.",</v>
+      </c>
+      <c r="G59" s="10" t="str">
+        <f>_xlfn.CONCAT(Sheet2!B$6,B59,Sheet2!B$7,B59,Sheet2!B$8)</f>
+        <v>$("[data-lang=home_greeting_text]").text(language.home_greeting_text);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>